<commit_message>
modified shuffleWord.py & maybe run correctly.
</commit_message>
<xml_diff>
--- a/WordList.xlsx
+++ b/WordList.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="shuffleWord" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="shuffleWord-ans" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,72 +16,135 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>a</t>
   </si>
   <si>
+    <t>え</t>
+  </si>
+  <si>
     <t>aa</t>
   </si>
   <si>
+    <t>ええ</t>
+  </si>
+  <si>
     <t>aaa</t>
   </si>
   <si>
+    <t>えええ</t>
+  </si>
+  <si>
     <t>aaaa</t>
   </si>
   <si>
+    <t>ええええ</t>
+  </si>
+  <si>
     <t>b</t>
   </si>
   <si>
+    <t>び</t>
+  </si>
+  <si>
     <t>bc</t>
   </si>
   <si>
+    <t>びし</t>
+  </si>
+  <si>
     <t>cat</t>
   </si>
   <si>
+    <t>猫</t>
+  </si>
+  <si>
     <t>hat</t>
   </si>
   <si>
+    <t>帽子</t>
+  </si>
+  <si>
     <t>hot</t>
   </si>
   <si>
+    <t>暑い</t>
+  </si>
+  <si>
     <t>not</t>
   </si>
   <si>
+    <t>〜でない</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
+    <t>１つもない</t>
+  </si>
+  <si>
     <t>bb</t>
   </si>
   <si>
+    <t>びび</t>
+  </si>
+  <si>
     <t>cc</t>
   </si>
   <si>
+    <t>しし</t>
+  </si>
+  <si>
     <t>dd</t>
   </si>
   <si>
+    <t>でで</t>
+  </si>
+  <si>
     <t>ee</t>
   </si>
   <si>
+    <t>いい</t>
+  </si>
+  <si>
     <t>ff</t>
   </si>
   <si>
+    <t>ふふ</t>
+  </si>
+  <si>
     <t>gg</t>
   </si>
   <si>
+    <t>じじ</t>
+  </si>
+  <si>
     <t>robot</t>
   </si>
   <si>
+    <t>ロボット</t>
+  </si>
+  <si>
     <t>dog</t>
   </si>
   <si>
+    <t>犬</t>
+  </si>
+  <si>
     <t>word</t>
   </si>
   <si>
+    <t>単語</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
     <t>Word</t>
+  </si>
+  <si>
+    <t>Ans</t>
   </si>
 </sst>
 </file>
@@ -145,11 +209,14 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
@@ -458,235 +525,295 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B2:B21 A1"/>
+      <selection activeCell="C21" activeCellId="0" pane="topLeft" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="3" width="12.2747747747748"/>
+    <col customWidth="1" max="1025" min="1" style="2" width="8.581081081081081"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.75" r="1" s="3" spans="1:3">
+    <row customHeight="1" ht="15.75" r="1" s="4" spans="1:4">
       <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="n">
-        <v>0.7625948660928352</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="2" s="3" spans="1:3">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="n">
+        <v>0.1639097948720433</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="2" s="4" spans="1:4">
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0.7245930961963325</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="3" s="3" spans="1:3">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0.0829102206592518</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="3" s="4" spans="1:4">
       <c r="A3" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>0.4721131158295511</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="4" s="3" spans="1:3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0.04354317377854944</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="4" spans="1:4">
       <c r="A4" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0.4716392625788569</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="5" s="3" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0.2149138675851595</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="4" spans="1:4">
       <c r="A5" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>0.1520997007403795</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="6" s="3" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0.6469913546123741</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="4" spans="1:4">
       <c r="A6" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>0.183362395907115</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="7" s="3" spans="1:3">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0.2061517477418859</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="4" spans="1:4">
       <c r="A7" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>0.3798504917674946</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="8" s="3" spans="1:3">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0.870965882966497</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" s="4" spans="1:4">
       <c r="A8" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>0.3304059857353366</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="9" s="3" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0.3009903093700209</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" s="4" spans="1:4">
       <c r="A9" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>0.03698601406304769</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="10" s="3" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0.1412223648937719</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="4" spans="1:4">
       <c r="A10" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>0.4315053978362619</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="11" s="3" spans="1:3">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0.7830808663629975</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" s="4" spans="1:4">
       <c r="A11" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>0.5007909728699637</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="12" s="3" spans="1:3">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0.06486449013155626</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="12" s="4" spans="1:4">
       <c r="A12" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>0.5510823725792278</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="13" s="3" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0.8010032180472988</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="13" s="4" spans="1:4">
       <c r="A13" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>0.7037802194241004</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="14" s="3" spans="1:3">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0.5863964369569264</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" s="4" spans="1:4">
       <c r="A14" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>0.8293820643915601</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="15" s="3" spans="1:3">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0.08281089167279354</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="4" spans="1:4">
       <c r="A15" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>0.6640317760757639</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="16" s="3" spans="1:3">
+        <v>28</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0.2202054843997382</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" s="4" spans="1:4">
       <c r="A16" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>0.4470276825887909</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="17" s="3" spans="1:3">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0.2074474693987007</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" s="4" spans="1:4">
       <c r="A17" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>0.2419375324895362</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="18" s="3" spans="1:3">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0.9821946726517806</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="18" s="4" spans="1:4">
       <c r="A18" s="1" t="n">
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>0.4504833205219084</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="19" s="3" spans="1:3">
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0.4132732627342857</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" s="4" spans="1:4">
       <c r="A19" s="1" t="n">
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>0.6425667942794761</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="20" s="3" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0.7772848813636258</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="20" s="4" spans="1:4">
       <c r="A20" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>0.9474810480935191</v>
+        <v>38</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0.9695341830492493</v>
       </c>
     </row>
   </sheetData>
@@ -702,180 +829,449 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="2" width="8.581081081081081"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="12.8" r="1" s="4" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="2" s="4" spans="1:3">
+      <c r="A2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="3" s="4" spans="1:3">
+      <c r="A3" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="4" s="4" spans="1:3">
+      <c r="A4" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="5" s="4" spans="1:3">
+      <c r="A5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="6" s="4" spans="1:3">
+      <c r="A6" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="7" s="4" spans="1:3">
+      <c r="A7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="8" s="4" spans="1:3">
+      <c r="A8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="9" s="4" spans="1:3">
+      <c r="A9" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="10" s="4" spans="1:3">
+      <c r="A10" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="11" s="4" spans="1:3">
+      <c r="A11" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="12" s="4" spans="1:3">
+      <c r="A12" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="13" s="4" spans="1:3">
+      <c r="A13" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="14" s="4" spans="1:3">
+      <c r="A14" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="15" s="4" spans="1:3">
+      <c r="A15" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="16" s="4" spans="1:3">
+      <c r="A16" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="17" s="4" spans="1:3">
+      <c r="A17" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="18" s="4" spans="1:3">
+      <c r="A18" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="19" s="4" spans="1:3">
+      <c r="A19" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="20" s="4" spans="1:3">
+      <c r="A20" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="21" s="4" spans="1:3">
+      <c r="A21" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <headerFooter differentFirst="0" differentOddEven="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12ページ &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2:B21"/>
+      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="2" width="10.0135135135135"/>
+  </cols>
   <sheetData>
-    <row customHeight="1" ht="12.8" r="1" s="3" spans="1:2">
-      <c r="A1" s="0" t="s">
+    <row customHeight="1" ht="12.8" r="1" s="4" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="2" s="4" spans="1:3">
+      <c r="A2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="3" s="4" spans="1:3">
+      <c r="A3" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row customHeight="1" ht="12.8" r="2" s="3" spans="1:2">
-      <c r="A2" s="0" t="n">
+    <row customHeight="1" ht="12.8" r="4" s="4" spans="1:3">
+      <c r="A4" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="5" s="4" spans="1:3">
+      <c r="A5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="6" s="4" spans="1:3">
+      <c r="A6" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="7" s="4" spans="1:3">
+      <c r="A7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="8" s="4" spans="1:3">
+      <c r="A8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="9" s="4" spans="1:3">
+      <c r="A9" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="10" s="4" spans="1:3">
+      <c r="A10" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="11" s="4" spans="1:3">
+      <c r="A11" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="12" s="4" spans="1:3">
+      <c r="A12" s="2" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="3" s="3" spans="1:2">
-      <c r="A3" s="0" t="n">
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="13" s="4" spans="1:3">
+      <c r="A13" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="14" s="4" spans="1:3">
+      <c r="A14" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="15" s="4" spans="1:3">
+      <c r="A15" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="4" s="3" spans="1:2">
-      <c r="A4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="5" s="3" spans="1:2">
-      <c r="A5" s="0" t="n">
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="16" s="4" spans="1:3">
+      <c r="A16" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="17" s="4" spans="1:3">
+      <c r="A17" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="18" s="4" spans="1:3">
+      <c r="A18" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="19" s="4" spans="1:3">
+      <c r="A19" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="20" s="4" spans="1:3">
+      <c r="A20" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="21" s="4" spans="1:3">
+      <c r="A21" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="6" s="3" spans="1:2">
-      <c r="A6" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="7" s="3" spans="1:2">
-      <c r="A7" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="8" s="3" spans="1:2">
-      <c r="A8" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="9" s="3" spans="1:2">
-      <c r="A9" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="10" s="3" spans="1:2">
-      <c r="A10" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="11" s="3" spans="1:2">
-      <c r="A11" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="12" s="3" spans="1:2">
-      <c r="A12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="13" s="3" spans="1:2">
-      <c r="A13" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="14" s="3" spans="1:2">
-      <c r="A14" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="15" s="3" spans="1:2">
-      <c r="A15" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="16" s="3" spans="1:2">
-      <c r="A16" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="17" s="3" spans="1:2">
-      <c r="A17" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="18" s="3" spans="1:2">
-      <c r="A18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="19" s="3" spans="1:2">
-      <c r="A19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="20" s="3" spans="1:2">
-      <c r="A20" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="21" s="3" spans="1:2">
-      <c r="A21" s="0" t="n">
-        <v>20</v>
-      </c>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>